<commit_message>
await asyncio.sleep(2) for zip input function
</commit_message>
<xml_diff>
--- a/test_amaz.xlsx
+++ b/test_amaz.xlsx
@@ -11,18 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="&quot;Aptos Narrow&quot;, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="12.0"/>
-        <u/>
-      </rPr>
-      <t>https://www.amazon.com/dp/B0CLYV18R5</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <r>
       <rPr>
@@ -94,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -102,6 +91,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
       <u/>
       <sz val="12.0"/>
       <color rgb="FF0000FF"/>
@@ -112,13 +106,29 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FFEEF0FF"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F1F1F"/>
+        <bgColor rgb="FF1F1F1F"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -135,7 +145,16 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,56 +373,65 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B2" s="3">
         <v>94513.0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="3">
         <v>60085.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="3">
+        <v>10010.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="4">
+        <v>73301.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="5">
+        <v>89001.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="B7" s="3">
+        <v>60085.0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A1"/>
-    <hyperlink r:id="rId2" ref="A2"/>
-    <hyperlink r:id="rId3" ref="A3"/>
-    <hyperlink r:id="rId4" ref="A4"/>
-    <hyperlink r:id="rId5" ref="A5"/>
-    <hyperlink r:id="rId6" ref="A6"/>
-    <hyperlink r:id="rId7" ref="A7"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>